<commit_message>
Path before imports added
</commit_message>
<xml_diff>
--- a/Data/Wyniki.xlsx
+++ b/Data/Wyniki.xlsx
@@ -1,43 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="bitcoin_LGBM_łączne" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="bitcoin_Base" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,26 +46,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -330,13 +399,226 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Annualized Return Compounded</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Annualized Standard Deviation</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Maximum drawdown</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Information Ratio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>-29.459999999999997%</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>77.98%</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>74.53%</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-37.769999999999996%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>-46.949999999999996%</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>77.98%</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>74.0%</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-60.209999999999994%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-31.69%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>77.98%</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>74.68%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-40.64%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>-46.83%</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>77.98%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>72.34%</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-60.06%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Annualized Return Compounded</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Annualized Standard Deviation</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Maximum drawdown</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Information Ratio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>-39.35%</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>77.98%</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>74.33%</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-50.470000000000006%</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>